<commit_message>
added project marks and attendance for cse 208 section 1
</commit_message>
<xml_diff>
--- a/FALL 19/CSE 208/results_cse208_sec1.xlsx
+++ b/FALL 19/CSE 208/results_cse208_sec1.xlsx
@@ -3,17 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E257AC53-EC1A-4D9D-9182-784D92077D7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363043A2-E490-4F0B-AF30-1F4E3C7D8FD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="quiz1" sheetId="1" r:id="rId1"/>
-    <sheet name="quiz2" sheetId="4" r:id="rId2"/>
-    <sheet name="quiz_final" sheetId="5" r:id="rId3"/>
-    <sheet name="mid" sheetId="2" r:id="rId4"/>
-    <sheet name="final" sheetId="3" r:id="rId5"/>
+    <sheet name="attendance" sheetId="6" r:id="rId1"/>
+    <sheet name="quiz1" sheetId="1" r:id="rId2"/>
+    <sheet name="quiz2" sheetId="4" r:id="rId3"/>
+    <sheet name="quiz_final" sheetId="5" r:id="rId4"/>
+    <sheet name="mid" sheetId="2" r:id="rId5"/>
+    <sheet name="final" sheetId="3" r:id="rId6"/>
+    <sheet name="project" sheetId="7" r:id="rId7"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId8"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -135,6 +140,18 @@
   </si>
   <si>
     <t>Converted_Total</t>
+  </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Present</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Code</t>
   </si>
 </sst>
 </file>
@@ -292,11 +309,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -370,12 +388,47 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{092E97F7-1693-4CB9-A1C9-BDE591DA97C5}"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="20">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -558,46 +611,8 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
+        <condense val="0"/>
+        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -627,6 +642,170 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="B2">
+            <v>183014079</v>
+          </cell>
+          <cell r="D2">
+            <v>183014079</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3">
+            <v>183014021</v>
+          </cell>
+          <cell r="D3">
+            <v>183014021</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>151014050</v>
+          </cell>
+          <cell r="D4">
+            <v>151014050</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>181014073</v>
+          </cell>
+          <cell r="C6">
+            <v>8.5</v>
+          </cell>
+          <cell r="D6">
+            <v>181014073</v>
+          </cell>
+          <cell r="E6">
+            <v>6.5</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7">
+            <v>161014055</v>
+          </cell>
+          <cell r="C7">
+            <v>8.5</v>
+          </cell>
+          <cell r="D7">
+            <v>161014055</v>
+          </cell>
+          <cell r="E7">
+            <v>6.5</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8">
+            <v>181014069</v>
+          </cell>
+          <cell r="C8">
+            <v>8.5</v>
+          </cell>
+          <cell r="D8">
+            <v>181014069</v>
+          </cell>
+          <cell r="E8">
+            <v>6.5</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10">
+            <v>182014036</v>
+          </cell>
+          <cell r="D10">
+            <v>182014036</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11">
+            <v>182014035</v>
+          </cell>
+          <cell r="D11">
+            <v>182014035</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12">
+            <v>182014003</v>
+          </cell>
+          <cell r="D12">
+            <v>182014003</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13">
+            <v>141014039</v>
+          </cell>
+          <cell r="D13">
+            <v>141014039</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15">
+            <v>173014003</v>
+          </cell>
+          <cell r="C15">
+            <v>9.5</v>
+          </cell>
+          <cell r="D15">
+            <v>173014003</v>
+          </cell>
+          <cell r="E15">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16">
+            <v>173014050</v>
+          </cell>
+          <cell r="C16">
+            <v>9.5</v>
+          </cell>
+          <cell r="D16">
+            <v>173014050</v>
+          </cell>
+          <cell r="E16">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17">
+            <v>182014006</v>
+          </cell>
+          <cell r="C17">
+            <v>9.5</v>
+          </cell>
+          <cell r="D17">
+            <v>182014006</v>
+          </cell>
+          <cell r="E17">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19">
+            <v>181014124</v>
+          </cell>
+          <cell r="D19">
+            <v>181014124</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -949,11 +1128,492 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7CB968-5C40-4FB2-AF7A-5928E1DBC66A}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="8" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>141014039</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="29">
+        <v>22</v>
+      </c>
+      <c r="D2" s="29">
+        <v>11</v>
+      </c>
+      <c r="E2" s="29">
+        <f>C2-D2</f>
+        <v>11</v>
+      </c>
+      <c r="F2" s="29">
+        <f>ROUNDUP((E2/C2)*F$16,0)</f>
+        <v>5</v>
+      </c>
+      <c r="G2" s="24">
+        <f>(F2/F$16)*100</f>
+        <v>50</v>
+      </c>
+      <c r="H2" s="21" t="str">
+        <f>IF(G2&gt;94,"A+",IF(G2&gt;84,"A",IF(G2&gt;79,"A-",IF(G2&gt;74,"B+",IF(G2&gt;69,"B",IF(G2&gt;64,"B-",IF(G2&gt;59,"C+",IF(G2&gt;54,"C",IF(G2&gt;49,"D","F")))))))))</f>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>151014050</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="17">
+        <v>14</v>
+      </c>
+      <c r="D3" s="17">
+        <v>14</v>
+      </c>
+      <c r="E3" s="29">
+        <f t="shared" ref="E3:E15" si="0">C3-D3</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="29">
+        <f t="shared" ref="F3:F15" si="1">ROUNDUP((E3/C3)*F$16,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="24">
+        <f t="shared" ref="G3:G15" si="2">(F3/F$16)*100</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="21" t="str">
+        <f t="shared" ref="H3:H15" si="3">IF(G3&gt;94,"A+",IF(G3&gt;84,"A",IF(G3&gt;79,"A-",IF(G3&gt;74,"B+",IF(G3&gt;69,"B",IF(G3&gt;64,"B-",IF(G3&gt;59,"C+",IF(G3&gt;54,"C",IF(G3&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>161014055</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="17">
+        <v>22</v>
+      </c>
+      <c r="D4" s="17">
+        <v>8</v>
+      </c>
+      <c r="E4" s="29">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F4" s="29">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G4" s="24">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H4" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>173014003</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="17">
+        <v>22</v>
+      </c>
+      <c r="D5" s="17">
+        <v>5</v>
+      </c>
+      <c r="E5" s="29">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="F5" s="29">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G5" s="24">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H5" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>173014050</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="17">
+        <v>22</v>
+      </c>
+      <c r="D6" s="33">
+        <v>2</v>
+      </c>
+      <c r="E6" s="29">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F6" s="29">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G6" s="24">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H6" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>181014069</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="33">
+        <v>18</v>
+      </c>
+      <c r="D7" s="33">
+        <v>7</v>
+      </c>
+      <c r="E7" s="29">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F7" s="29">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G7" s="24">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H7" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>181014073</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="17">
+        <v>22</v>
+      </c>
+      <c r="D8" s="33">
+        <v>8</v>
+      </c>
+      <c r="E8" s="29">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F8" s="29">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G8" s="24">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H8" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>181014124</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="17">
+        <v>22</v>
+      </c>
+      <c r="D9" s="33">
+        <v>7</v>
+      </c>
+      <c r="E9" s="29">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F9" s="29">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G9" s="24">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H9" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>182014003</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="17">
+        <v>22</v>
+      </c>
+      <c r="D10" s="33">
+        <v>3</v>
+      </c>
+      <c r="E10" s="29">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F10" s="29">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G10" s="24">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H10" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>182014006</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="17">
+        <v>22</v>
+      </c>
+      <c r="D11" s="33">
+        <v>2</v>
+      </c>
+      <c r="E11" s="29">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F11" s="29">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G11" s="24">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H11" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>182014035</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="17">
+        <v>22</v>
+      </c>
+      <c r="D12" s="33">
+        <v>12</v>
+      </c>
+      <c r="E12" s="29">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F12" s="29">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G12" s="24">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="H12" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>182014036</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="17">
+        <v>22</v>
+      </c>
+      <c r="D13" s="33">
+        <v>12</v>
+      </c>
+      <c r="E13" s="29">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F13" s="29">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G13" s="24">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="H13" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>183014021</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="17">
+        <v>22</v>
+      </c>
+      <c r="D14" s="33">
+        <v>14</v>
+      </c>
+      <c r="E14" s="29">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F14" s="29">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G14" s="24">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="H14" s="21" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="12">
+        <v>183014079</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="32">
+        <v>22</v>
+      </c>
+      <c r="D15" s="32">
+        <v>6</v>
+      </c>
+      <c r="E15" s="30">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F15" s="30">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G15" s="22">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H15" s="23" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:E2 E3:E15">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="greaterThan">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H15">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I15"/>
+      <selection activeCell="A2" sqref="A2:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1574,22 +2234,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C15">
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E15">
-    <cfRule type="cellIs" dxfId="19" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G15">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L15">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1598,7 +2258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892DCAF5-50B4-4CC9-862F-26311DF5AD1C}">
   <dimension ref="A1:J15"/>
   <sheetViews>
@@ -2117,17 +2777,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C15">
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E15">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J15">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2135,7 +2795,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A081D27-E9DB-448D-BF32-6D25191E253E}">
   <dimension ref="A1:L36"/>
   <sheetViews>
@@ -2251,7 +2911,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="29">
-        <f t="shared" ref="G3:H36" si="0">C3+E3</f>
+        <f t="shared" ref="G3:H15" si="0">C3+E3</f>
         <v>0</v>
       </c>
       <c r="H3" s="29">
@@ -2259,18 +2919,18 @@
         <v>40</v>
       </c>
       <c r="I3" s="29">
-        <f t="shared" ref="I3:I36" si="1">(G3/H3)*J3</f>
+        <f t="shared" ref="I3:I15" si="1">(G3/H3)*J3</f>
         <v>0</v>
       </c>
       <c r="J3" s="29">
         <v>20</v>
       </c>
       <c r="K3" s="24">
-        <f t="shared" ref="K3:K36" si="2">(I3/J3)*100</f>
+        <f t="shared" ref="K3:K15" si="2">(I3/J3)*100</f>
         <v>0</v>
       </c>
       <c r="L3" s="21" t="str">
-        <f t="shared" ref="L3:L36" si="3">IF(K3&gt;94,"A+",IF(K3&gt;84,"A",IF(K3&gt;79,"A-",IF(K3&gt;74,"B+",IF(K3&gt;69,"B",IF(K3&gt;64,"B-",IF(K3&gt;59,"C+",IF(K3&gt;54,"C",IF(K3&gt;49,"D","F")))))))))</f>
+        <f t="shared" ref="L3:L15" si="3">IF(K3&gt;94,"A+",IF(K3&gt;84,"A",IF(K3&gt;79,"A-",IF(K3&gt;74,"B+",IF(K3&gt;69,"B",IF(K3&gt;64,"B-",IF(K3&gt;59,"C+",IF(K3&gt;54,"C",IF(K3&gt;49,"D","F")))))))))</f>
         <v>F</v>
       </c>
     </row>
@@ -3086,7 +3746,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L36">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3094,7 +3754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N15"/>
   <sheetViews>
@@ -3776,27 +4436,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C15">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E15">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G15">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I15">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
       <formula>$J$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N15">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3805,11 +4465,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -4438,30 +5098,607 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C15">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E15">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G15">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I15">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>$J$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N15">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB8A15D-7917-46AD-890F-E9C4AF848589}">
+  <dimension ref="A1:G48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.77734375" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="7" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="37">
+        <v>141014039</v>
+      </c>
+      <c r="C2" s="38">
+        <f>VLOOKUP(B2,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="38">
+        <f>VLOOKUP(B2,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="38">
+        <f t="shared" ref="E2:E16" si="0">C2+D2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="38">
+        <f>(E2/E$16)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="39" t="str">
+        <f t="shared" ref="G2:G15" si="1">IF(F2&gt;94,"A+",IF(F2&gt;84,"A",IF(F2&gt;79,"A-",IF(F2&gt;74,"B+",IF(F2&gt;69,"B",IF(F2&gt;64,"B-",IF(F2&gt;59,"C+",IF(F2&gt;54,"C",IF(F2&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="37">
+        <v>151014050</v>
+      </c>
+      <c r="C3" s="38">
+        <f>VLOOKUP(B3,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="38">
+        <f>VLOOKUP(B3,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="38">
+        <f t="shared" ref="F3:F15" si="2">(E3/E$16)*100</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="37">
+        <v>161014055</v>
+      </c>
+      <c r="C4" s="38">
+        <f>VLOOKUP(B4,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>8.5</v>
+      </c>
+      <c r="D4" s="38">
+        <f>VLOOKUP(B4,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>6.5</v>
+      </c>
+      <c r="E4" s="38">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F4" s="38">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="G4" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>B+</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="37">
+        <v>173014003</v>
+      </c>
+      <c r="C5" s="38">
+        <f>VLOOKUP(B5,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>9.5</v>
+      </c>
+      <c r="D5" s="38">
+        <f>VLOOKUP(B5,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="E5" s="38">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
+      <c r="F5" s="38">
+        <f t="shared" si="2"/>
+        <v>82.5</v>
+      </c>
+      <c r="G5" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="37">
+        <v>173014050</v>
+      </c>
+      <c r="C6" s="38">
+        <f>VLOOKUP(B6,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>9.5</v>
+      </c>
+      <c r="D6" s="38">
+        <f>VLOOKUP(B6,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="E6" s="38">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
+      <c r="F6" s="38">
+        <f t="shared" si="2"/>
+        <v>82.5</v>
+      </c>
+      <c r="G6" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="37">
+        <v>181014069</v>
+      </c>
+      <c r="C7" s="38">
+        <f>VLOOKUP(B7,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>8.5</v>
+      </c>
+      <c r="D7" s="38">
+        <f>VLOOKUP(B7,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>6.5</v>
+      </c>
+      <c r="E7" s="38">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F7" s="38">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="G7" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>B+</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="37">
+        <v>181014073</v>
+      </c>
+      <c r="C8" s="38">
+        <f>VLOOKUP(B8,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>8.5</v>
+      </c>
+      <c r="D8" s="38">
+        <f>VLOOKUP(B8,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>6.5</v>
+      </c>
+      <c r="E8" s="38">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F8" s="38">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="G8" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>B+</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="37">
+        <v>181014124</v>
+      </c>
+      <c r="C9" s="38">
+        <f>VLOOKUP(B9,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="38">
+        <f>VLOOKUP(B9,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="37">
+        <v>182014003</v>
+      </c>
+      <c r="C10" s="38">
+        <f>VLOOKUP(B10,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="38">
+        <f>VLOOKUP(B10,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="37">
+        <v>182014006</v>
+      </c>
+      <c r="C11" s="38">
+        <f>VLOOKUP(B11,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>9.5</v>
+      </c>
+      <c r="D11" s="38">
+        <f>VLOOKUP(B11,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="E11" s="38">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
+      <c r="F11" s="38">
+        <f t="shared" si="2"/>
+        <v>82.5</v>
+      </c>
+      <c r="G11" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="37">
+        <v>182014035</v>
+      </c>
+      <c r="C12" s="38">
+        <f>VLOOKUP(B12,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="38">
+        <f>VLOOKUP(B12,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="37">
+        <v>182014036</v>
+      </c>
+      <c r="C13" s="38">
+        <f>VLOOKUP(B13,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="38">
+        <f>VLOOKUP(B13,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="37">
+        <v>183014021</v>
+      </c>
+      <c r="C14" s="38">
+        <f>VLOOKUP(B14,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="38">
+        <f>VLOOKUP(B14,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="39" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="41">
+        <v>183014079</v>
+      </c>
+      <c r="C15" s="42">
+        <f>VLOOKUP(B15,[1]Sheet1!B$2:C$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="42">
+        <f>VLOOKUP(B15,[1]Sheet1!D$2:E$19,2,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="42">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="44"/>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16" s="38">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="44"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="44"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="44"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="44"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="44"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="44"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="44"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="44"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="44"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="44"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+      <c r="B27" s="44"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="44"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="44"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="44"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="44"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="44"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+      <c r="B33" s="44"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
+      <c r="B34" s="44"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="44"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="44"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="44"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="44"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="44"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
+      <c r="B40" s="44"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="44"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="2"/>
+      <c r="B42" s="44"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="44"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="2"/>
+      <c r="B44" s="44"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="44"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="44"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="44"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="2"/>
+      <c r="B48" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>